<commit_message>
major refactoring of the code
</commit_message>
<xml_diff>
--- a/data/projects.xlsx
+++ b/data/projects.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>code</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>Uldis bērzkrogs</t>
+  </si>
+  <si>
+    <t>Agni salons</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -1190,13 +1196,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="5.85714285714286" customWidth="1"/>
     <col min="2" max="2" width="12.1428571428571" customWidth="1"/>
@@ -1247,6 +1253,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>914</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>